<commit_message>
generated file changes during testing
</commit_message>
<xml_diff>
--- a/antha/examples/workflows/AccuracyTest/AccuracytestPostMixHVoutput_test.xlsx
+++ b/antha/examples/workflows/AccuracyTest/AccuracytestPostMixHVoutput_test.xlsx
@@ -57,42 +57,42 @@
     <t>Plate WellYStart</t>
   </si>
   <si>
+    <t>LHPolicy_POST_MIX</t>
+  </si>
+  <si>
+    <t>LHPolicy_POST_MIX_VOLUME</t>
+  </si>
+  <si>
+    <t>LHPolicy_ASPSPEED</t>
+  </si>
+  <si>
+    <t>LHPolicy_CAN_MSA</t>
+  </si>
+  <si>
+    <t>LHPolicy_DSPZOFFSET</t>
+  </si>
+  <si>
+    <t>LHPolicy_TIP_REUSE_LIMIT</t>
+  </si>
+  <si>
     <t>LHPolicy_POST_MIX_RATE</t>
   </si>
   <si>
+    <t>LHPolicy_DSPSPEED</t>
+  </si>
+  <si>
     <t>LHPolicy_CAN_MULTI</t>
   </si>
   <si>
-    <t>LHPolicy_CAN_MSA</t>
-  </si>
-  <si>
     <t>LHPolicy_CAN_SDD</t>
   </si>
   <si>
+    <t>LHPolicy_DSPREFERENCE</t>
+  </si>
+  <si>
     <t>LHPolicy_NO_AIR_DISPENSE</t>
   </si>
   <si>
-    <t>LHPolicy_DSPZOFFSET</t>
-  </si>
-  <si>
-    <t>LHPolicy_TIP_REUSE_LIMIT</t>
-  </si>
-  <si>
-    <t>LHPolicy_POST_MIX</t>
-  </si>
-  <si>
-    <t>LHPolicy_POST_MIX_VOLUME</t>
-  </si>
-  <si>
-    <t>LHPolicy_ASPSPEED</t>
-  </si>
-  <si>
-    <t>LHPolicy_DSPSPEED</t>
-  </si>
-  <si>
-    <t>LHPolicy_DSPREFERENCE</t>
-  </si>
-  <si>
     <t>tartrazine</t>
   </si>
   <si>
@@ -102,7 +102,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>K6</t>
+    <t>E10</t>
   </si>
   <si>
     <t>PostMix</t>
@@ -120,115 +120,115 @@
     <t>2</t>
   </si>
   <si>
-    <t>P14</t>
+    <t>L4</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>G13</t>
+    <t>L7</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>I12</t>
+  </si>
+  <si>
+    <t>30.000ul</t>
+  </si>
+  <si>
+    <t>N5</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>N11</t>
+  </si>
+  <si>
+    <t>F15</t>
+  </si>
+  <si>
     <t>N8</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>F11</t>
-  </si>
-  <si>
-    <t>30.000ul</t>
-  </si>
-  <si>
-    <t>N7</t>
-  </si>
-  <si>
-    <t>O15</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
-    <t>B10</t>
-  </si>
-  <si>
-    <t>G16</t>
-  </si>
-  <si>
     <t>35.000ul</t>
   </si>
   <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>H15</t>
-  </si>
-  <si>
-    <t>J12</t>
-  </si>
-  <si>
-    <t>K5</t>
-  </si>
-  <si>
-    <t>M4</t>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>I4</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>M12</t>
+  </si>
+  <si>
+    <t>M14</t>
   </si>
   <si>
     <t>40.000ul</t>
   </si>
   <si>
-    <t>N5</t>
-  </si>
-  <si>
-    <t>O2</t>
-  </si>
-  <si>
-    <t>P15</t>
+    <t>O14</t>
+  </si>
+  <si>
+    <t>K13</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>I13</t>
   </si>
   <si>
     <t>J6</t>
   </si>
   <si>
-    <t>P16</t>
-  </si>
-  <si>
     <t>45.000ul</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>F13</t>
-  </si>
-  <si>
-    <t>M7</t>
-  </si>
-  <si>
-    <t>K13</t>
-  </si>
-  <si>
-    <t>G12</t>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>H11</t>
+  </si>
+  <si>
+    <t>I8</t>
+  </si>
+  <si>
+    <t>J10</t>
   </si>
   <si>
     <t>50.000ul</t>
   </si>
   <si>
-    <t>H8</t>
-  </si>
-  <si>
-    <t>F5</t>
-  </si>
-  <si>
-    <t>M11</t>
-  </si>
-  <si>
-    <t>L6</t>
+    <t>O12</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>L5</t>
   </si>
   <si>
     <t>M3</t>
+  </si>
+  <si>
+    <t>H12</t>
   </si>
 </sst>
 </file>
@@ -753,40 +753,40 @@
         <v>-2.5</v>
       </c>
       <c r="N2">
-        <v>3.74</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2">
+        <v>3.74</v>
       </c>
       <c r="Q2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2">
+        <v>0.5</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>3.74</v>
+      </c>
+      <c r="U2">
+        <v>3.74</v>
+      </c>
+      <c r="V2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
         <v>32</v>
-      </c>
-      <c r="S2">
-        <v>0.5</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>3</v>
-      </c>
-      <c r="V2">
-        <v>10</v>
-      </c>
-      <c r="W2">
-        <v>3.74</v>
-      </c>
-      <c r="X2">
-        <v>3.74</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -830,40 +830,40 @@
         <v>-2.5</v>
       </c>
       <c r="N3">
-        <v>3.74</v>
-      </c>
-      <c r="O3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>3.74</v>
       </c>
       <c r="Q3" t="s">
         <v>31</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3">
+        <v>0.5</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>3.74</v>
+      </c>
+      <c r="U3">
+        <v>3.74</v>
+      </c>
+      <c r="V3" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" t="s">
+        <v>31</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="s">
         <v>32</v>
-      </c>
-      <c r="S3">
-        <v>0.5</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>3</v>
-      </c>
-      <c r="V3">
-        <v>10</v>
-      </c>
-      <c r="W3">
-        <v>3.74</v>
-      </c>
-      <c r="X3">
-        <v>3.74</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -907,40 +907,40 @@
         <v>-2.5</v>
       </c>
       <c r="N4">
-        <v>3.74</v>
-      </c>
-      <c r="O4" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+      <c r="P4">
+        <v>3.74</v>
       </c>
       <c r="Q4" t="s">
         <v>31</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4">
+        <v>0.5</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>3.74</v>
+      </c>
+      <c r="U4">
+        <v>3.74</v>
+      </c>
+      <c r="V4" t="s">
+        <v>31</v>
+      </c>
+      <c r="W4" t="s">
+        <v>31</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="s">
         <v>32</v>
-      </c>
-      <c r="S4">
-        <v>0.5</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>3</v>
-      </c>
-      <c r="V4">
-        <v>10</v>
-      </c>
-      <c r="W4">
-        <v>3.74</v>
-      </c>
-      <c r="X4">
-        <v>3.74</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -984,40 +984,40 @@
         <v>-2.5</v>
       </c>
       <c r="N5">
-        <v>3.74</v>
-      </c>
-      <c r="O5" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>3.74</v>
       </c>
       <c r="Q5" t="s">
         <v>31</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5">
+        <v>0.5</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>3.74</v>
+      </c>
+      <c r="U5">
+        <v>3.74</v>
+      </c>
+      <c r="V5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
         <v>32</v>
-      </c>
-      <c r="S5">
-        <v>0.5</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>3</v>
-      </c>
-      <c r="V5">
-        <v>10</v>
-      </c>
-      <c r="W5">
-        <v>3.74</v>
-      </c>
-      <c r="X5">
-        <v>3.74</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1061,40 +1061,40 @@
         <v>-2.5</v>
       </c>
       <c r="N6">
-        <v>3.74</v>
-      </c>
-      <c r="O6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P6" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>10</v>
+      </c>
+      <c r="P6">
+        <v>3.74</v>
       </c>
       <c r="Q6" t="s">
         <v>31</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6">
+        <v>0.5</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>3.74</v>
+      </c>
+      <c r="U6">
+        <v>3.74</v>
+      </c>
+      <c r="V6" t="s">
+        <v>31</v>
+      </c>
+      <c r="W6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
         <v>32</v>
-      </c>
-      <c r="S6">
-        <v>0.5</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>3</v>
-      </c>
-      <c r="V6">
-        <v>10</v>
-      </c>
-      <c r="W6">
-        <v>3.74</v>
-      </c>
-      <c r="X6">
-        <v>3.74</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1138,40 +1138,40 @@
         <v>-2.5</v>
       </c>
       <c r="N7">
-        <v>3.74</v>
-      </c>
-      <c r="O7" t="s">
-        <v>31</v>
-      </c>
-      <c r="P7" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>3.74</v>
       </c>
       <c r="Q7" t="s">
         <v>31</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7">
+        <v>0.5</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>3.74</v>
+      </c>
+      <c r="U7">
+        <v>3.74</v>
+      </c>
+      <c r="V7" t="s">
+        <v>31</v>
+      </c>
+      <c r="W7" t="s">
+        <v>31</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="s">
         <v>32</v>
-      </c>
-      <c r="S7">
-        <v>0.5</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>3</v>
-      </c>
-      <c r="V7">
-        <v>10</v>
-      </c>
-      <c r="W7">
-        <v>3.74</v>
-      </c>
-      <c r="X7">
-        <v>3.74</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1215,40 +1215,40 @@
         <v>-2.5</v>
       </c>
       <c r="N8">
-        <v>3.74</v>
-      </c>
-      <c r="O8" t="s">
-        <v>31</v>
-      </c>
-      <c r="P8" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <v>3.74</v>
       </c>
       <c r="Q8" t="s">
         <v>31</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8">
+        <v>0.5</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>3.74</v>
+      </c>
+      <c r="U8">
+        <v>3.74</v>
+      </c>
+      <c r="V8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="s">
         <v>32</v>
-      </c>
-      <c r="S8">
-        <v>0.5</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>3</v>
-      </c>
-      <c r="V8">
-        <v>10</v>
-      </c>
-      <c r="W8">
-        <v>3.74</v>
-      </c>
-      <c r="X8">
-        <v>3.74</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1292,40 +1292,40 @@
         <v>-2.5</v>
       </c>
       <c r="N9">
-        <v>3.74</v>
-      </c>
-      <c r="O9" t="s">
-        <v>31</v>
-      </c>
-      <c r="P9" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>10</v>
+      </c>
+      <c r="P9">
+        <v>3.74</v>
       </c>
       <c r="Q9" t="s">
         <v>31</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9">
+        <v>0.5</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>3.74</v>
+      </c>
+      <c r="U9">
+        <v>3.74</v>
+      </c>
+      <c r="V9" t="s">
+        <v>31</v>
+      </c>
+      <c r="W9" t="s">
+        <v>31</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="s">
         <v>32</v>
-      </c>
-      <c r="S9">
-        <v>0.5</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>3</v>
-      </c>
-      <c r="V9">
-        <v>10</v>
-      </c>
-      <c r="W9">
-        <v>3.74</v>
-      </c>
-      <c r="X9">
-        <v>3.74</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1369,40 +1369,40 @@
         <v>-2.5</v>
       </c>
       <c r="N10">
-        <v>3.74</v>
-      </c>
-      <c r="O10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P10" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <v>3.74</v>
       </c>
       <c r="Q10" t="s">
         <v>31</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10">
+        <v>0.5</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>3.74</v>
+      </c>
+      <c r="U10">
+        <v>3.74</v>
+      </c>
+      <c r="V10" t="s">
+        <v>31</v>
+      </c>
+      <c r="W10" t="s">
+        <v>31</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="s">
         <v>32</v>
-      </c>
-      <c r="S10">
-        <v>0.5</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>3</v>
-      </c>
-      <c r="V10">
-        <v>10</v>
-      </c>
-      <c r="W10">
-        <v>3.74</v>
-      </c>
-      <c r="X10">
-        <v>3.74</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1446,40 +1446,40 @@
         <v>-2.5</v>
       </c>
       <c r="N11">
-        <v>3.74</v>
-      </c>
-      <c r="O11" t="s">
-        <v>31</v>
-      </c>
-      <c r="P11" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>3.74</v>
       </c>
       <c r="Q11" t="s">
         <v>31</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11">
+        <v>0.5</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>3.74</v>
+      </c>
+      <c r="U11">
+        <v>3.74</v>
+      </c>
+      <c r="V11" t="s">
+        <v>31</v>
+      </c>
+      <c r="W11" t="s">
+        <v>31</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="s">
         <v>32</v>
-      </c>
-      <c r="S11">
-        <v>0.5</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>3</v>
-      </c>
-      <c r="V11">
-        <v>10</v>
-      </c>
-      <c r="W11">
-        <v>3.74</v>
-      </c>
-      <c r="X11">
-        <v>3.74</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1523,40 +1523,40 @@
         <v>-2.5</v>
       </c>
       <c r="N12">
-        <v>3.74</v>
-      </c>
-      <c r="O12" t="s">
-        <v>31</v>
-      </c>
-      <c r="P12" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <v>3.74</v>
       </c>
       <c r="Q12" t="s">
         <v>31</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12">
+        <v>0.5</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>3.74</v>
+      </c>
+      <c r="U12">
+        <v>3.74</v>
+      </c>
+      <c r="V12" t="s">
+        <v>31</v>
+      </c>
+      <c r="W12" t="s">
+        <v>31</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="s">
         <v>32</v>
-      </c>
-      <c r="S12">
-        <v>0.5</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>3</v>
-      </c>
-      <c r="V12">
-        <v>10</v>
-      </c>
-      <c r="W12">
-        <v>3.74</v>
-      </c>
-      <c r="X12">
-        <v>3.74</v>
-      </c>
-      <c r="Y12">
-        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1600,40 +1600,40 @@
         <v>-2.5</v>
       </c>
       <c r="N13">
-        <v>3.74</v>
-      </c>
-      <c r="O13" t="s">
-        <v>31</v>
-      </c>
-      <c r="P13" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>10</v>
+      </c>
+      <c r="P13">
+        <v>3.74</v>
       </c>
       <c r="Q13" t="s">
         <v>31</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13">
+        <v>0.5</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>3.74</v>
+      </c>
+      <c r="U13">
+        <v>3.74</v>
+      </c>
+      <c r="V13" t="s">
+        <v>31</v>
+      </c>
+      <c r="W13" t="s">
+        <v>31</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
         <v>32</v>
-      </c>
-      <c r="S13">
-        <v>0.5</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>3</v>
-      </c>
-      <c r="V13">
-        <v>10</v>
-      </c>
-      <c r="W13">
-        <v>3.74</v>
-      </c>
-      <c r="X13">
-        <v>3.74</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1677,40 +1677,40 @@
         <v>-2.5</v>
       </c>
       <c r="N14">
-        <v>3.74</v>
-      </c>
-      <c r="O14" t="s">
-        <v>31</v>
-      </c>
-      <c r="P14" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>10</v>
+      </c>
+      <c r="P14">
+        <v>3.74</v>
       </c>
       <c r="Q14" t="s">
         <v>31</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14">
+        <v>0.5</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>3.74</v>
+      </c>
+      <c r="U14">
+        <v>3.74</v>
+      </c>
+      <c r="V14" t="s">
+        <v>31</v>
+      </c>
+      <c r="W14" t="s">
+        <v>31</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
         <v>32</v>
-      </c>
-      <c r="S14">
-        <v>0.5</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>3</v>
-      </c>
-      <c r="V14">
-        <v>10</v>
-      </c>
-      <c r="W14">
-        <v>3.74</v>
-      </c>
-      <c r="X14">
-        <v>3.74</v>
-      </c>
-      <c r="Y14">
-        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1754,40 +1754,40 @@
         <v>-2.5</v>
       </c>
       <c r="N15">
-        <v>3.74</v>
-      </c>
-      <c r="O15" t="s">
-        <v>31</v>
-      </c>
-      <c r="P15" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="P15">
+        <v>3.74</v>
       </c>
       <c r="Q15" t="s">
         <v>31</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R15">
+        <v>0.5</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>3.74</v>
+      </c>
+      <c r="U15">
+        <v>3.74</v>
+      </c>
+      <c r="V15" t="s">
+        <v>31</v>
+      </c>
+      <c r="W15" t="s">
+        <v>31</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
         <v>32</v>
-      </c>
-      <c r="S15">
-        <v>0.5</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>3</v>
-      </c>
-      <c r="V15">
-        <v>10</v>
-      </c>
-      <c r="W15">
-        <v>3.74</v>
-      </c>
-      <c r="X15">
-        <v>3.74</v>
-      </c>
-      <c r="Y15">
-        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1831,40 +1831,40 @@
         <v>-2.5</v>
       </c>
       <c r="N16">
-        <v>3.74</v>
-      </c>
-      <c r="O16" t="s">
-        <v>31</v>
-      </c>
-      <c r="P16" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>3.74</v>
       </c>
       <c r="Q16" t="s">
         <v>31</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16">
+        <v>0.5</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>3.74</v>
+      </c>
+      <c r="U16">
+        <v>3.74</v>
+      </c>
+      <c r="V16" t="s">
+        <v>31</v>
+      </c>
+      <c r="W16" t="s">
+        <v>31</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="s">
         <v>32</v>
-      </c>
-      <c r="S16">
-        <v>0.5</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>3</v>
-      </c>
-      <c r="V16">
-        <v>10</v>
-      </c>
-      <c r="W16">
-        <v>3.74</v>
-      </c>
-      <c r="X16">
-        <v>3.74</v>
-      </c>
-      <c r="Y16">
-        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1908,40 +1908,40 @@
         <v>-2.5</v>
       </c>
       <c r="N17">
-        <v>3.74</v>
-      </c>
-      <c r="O17" t="s">
-        <v>31</v>
-      </c>
-      <c r="P17" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O17">
+        <v>10</v>
+      </c>
+      <c r="P17">
+        <v>3.74</v>
       </c>
       <c r="Q17" t="s">
         <v>31</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17">
+        <v>0.5</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>3.74</v>
+      </c>
+      <c r="U17">
+        <v>3.74</v>
+      </c>
+      <c r="V17" t="s">
+        <v>31</v>
+      </c>
+      <c r="W17" t="s">
+        <v>31</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="s">
         <v>32</v>
-      </c>
-      <c r="S17">
-        <v>0.5</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>3</v>
-      </c>
-      <c r="V17">
-        <v>10</v>
-      </c>
-      <c r="W17">
-        <v>3.74</v>
-      </c>
-      <c r="X17">
-        <v>3.74</v>
-      </c>
-      <c r="Y17">
-        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1985,40 +1985,40 @@
         <v>-2.5</v>
       </c>
       <c r="N18">
-        <v>3.74</v>
-      </c>
-      <c r="O18" t="s">
-        <v>31</v>
-      </c>
-      <c r="P18" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O18">
+        <v>10</v>
+      </c>
+      <c r="P18">
+        <v>3.74</v>
       </c>
       <c r="Q18" t="s">
         <v>31</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R18">
+        <v>0.5</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>3.74</v>
+      </c>
+      <c r="U18">
+        <v>3.74</v>
+      </c>
+      <c r="V18" t="s">
+        <v>31</v>
+      </c>
+      <c r="W18" t="s">
+        <v>31</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
         <v>32</v>
-      </c>
-      <c r="S18">
-        <v>0.5</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>3</v>
-      </c>
-      <c r="V18">
-        <v>10</v>
-      </c>
-      <c r="W18">
-        <v>3.74</v>
-      </c>
-      <c r="X18">
-        <v>3.74</v>
-      </c>
-      <c r="Y18">
-        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -2062,40 +2062,40 @@
         <v>-2.5</v>
       </c>
       <c r="N19">
-        <v>3.74</v>
-      </c>
-      <c r="O19" t="s">
-        <v>31</v>
-      </c>
-      <c r="P19" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>10</v>
+      </c>
+      <c r="P19">
+        <v>3.74</v>
       </c>
       <c r="Q19" t="s">
         <v>31</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R19">
+        <v>0.5</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>3.74</v>
+      </c>
+      <c r="U19">
+        <v>3.74</v>
+      </c>
+      <c r="V19" t="s">
+        <v>31</v>
+      </c>
+      <c r="W19" t="s">
+        <v>31</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="s">
         <v>32</v>
-      </c>
-      <c r="S19">
-        <v>0.5</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>3</v>
-      </c>
-      <c r="V19">
-        <v>10</v>
-      </c>
-      <c r="W19">
-        <v>3.74</v>
-      </c>
-      <c r="X19">
-        <v>3.74</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -2139,40 +2139,40 @@
         <v>-2.5</v>
       </c>
       <c r="N20">
-        <v>3.74</v>
-      </c>
-      <c r="O20" t="s">
-        <v>31</v>
-      </c>
-      <c r="P20" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O20">
+        <v>10</v>
+      </c>
+      <c r="P20">
+        <v>3.74</v>
       </c>
       <c r="Q20" t="s">
         <v>31</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R20">
+        <v>0.5</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>3.74</v>
+      </c>
+      <c r="U20">
+        <v>3.74</v>
+      </c>
+      <c r="V20" t="s">
+        <v>31</v>
+      </c>
+      <c r="W20" t="s">
+        <v>31</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="s">
         <v>32</v>
-      </c>
-      <c r="S20">
-        <v>0.5</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>3</v>
-      </c>
-      <c r="V20">
-        <v>10</v>
-      </c>
-      <c r="W20">
-        <v>3.74</v>
-      </c>
-      <c r="X20">
-        <v>3.74</v>
-      </c>
-      <c r="Y20">
-        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -2216,40 +2216,40 @@
         <v>-2.5</v>
       </c>
       <c r="N21">
-        <v>3.74</v>
-      </c>
-      <c r="O21" t="s">
-        <v>31</v>
-      </c>
-      <c r="P21" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O21">
+        <v>10</v>
+      </c>
+      <c r="P21">
+        <v>3.74</v>
       </c>
       <c r="Q21" t="s">
         <v>31</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21">
+        <v>0.5</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>3.74</v>
+      </c>
+      <c r="U21">
+        <v>3.74</v>
+      </c>
+      <c r="V21" t="s">
+        <v>31</v>
+      </c>
+      <c r="W21" t="s">
+        <v>31</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="s">
         <v>32</v>
-      </c>
-      <c r="S21">
-        <v>0.5</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>3</v>
-      </c>
-      <c r="V21">
-        <v>10</v>
-      </c>
-      <c r="W21">
-        <v>3.74</v>
-      </c>
-      <c r="X21">
-        <v>3.74</v>
-      </c>
-      <c r="Y21">
-        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2293,40 +2293,40 @@
         <v>-2.5</v>
       </c>
       <c r="N22">
-        <v>3.74</v>
-      </c>
-      <c r="O22" t="s">
-        <v>31</v>
-      </c>
-      <c r="P22" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O22">
+        <v>10</v>
+      </c>
+      <c r="P22">
+        <v>3.74</v>
       </c>
       <c r="Q22" t="s">
         <v>31</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22">
+        <v>0.5</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>3.74</v>
+      </c>
+      <c r="U22">
+        <v>3.74</v>
+      </c>
+      <c r="V22" t="s">
+        <v>31</v>
+      </c>
+      <c r="W22" t="s">
+        <v>31</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="s">
         <v>32</v>
-      </c>
-      <c r="S22">
-        <v>0.5</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>3</v>
-      </c>
-      <c r="V22">
-        <v>10</v>
-      </c>
-      <c r="W22">
-        <v>3.74</v>
-      </c>
-      <c r="X22">
-        <v>3.74</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2370,40 +2370,40 @@
         <v>-2.5</v>
       </c>
       <c r="N23">
-        <v>3.74</v>
-      </c>
-      <c r="O23" t="s">
-        <v>31</v>
-      </c>
-      <c r="P23" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O23">
+        <v>10</v>
+      </c>
+      <c r="P23">
+        <v>3.74</v>
       </c>
       <c r="Q23" t="s">
         <v>31</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R23">
+        <v>0.5</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>3.74</v>
+      </c>
+      <c r="U23">
+        <v>3.74</v>
+      </c>
+      <c r="V23" t="s">
+        <v>31</v>
+      </c>
+      <c r="W23" t="s">
+        <v>31</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="s">
         <v>32</v>
-      </c>
-      <c r="S23">
-        <v>0.5</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>3</v>
-      </c>
-      <c r="V23">
-        <v>10</v>
-      </c>
-      <c r="W23">
-        <v>3.74</v>
-      </c>
-      <c r="X23">
-        <v>3.74</v>
-      </c>
-      <c r="Y23">
-        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2447,40 +2447,40 @@
         <v>-2.5</v>
       </c>
       <c r="N24">
-        <v>3.74</v>
-      </c>
-      <c r="O24" t="s">
-        <v>31</v>
-      </c>
-      <c r="P24" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O24">
+        <v>10</v>
+      </c>
+      <c r="P24">
+        <v>3.74</v>
       </c>
       <c r="Q24" t="s">
         <v>31</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R24">
+        <v>0.5</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>3.74</v>
+      </c>
+      <c r="U24">
+        <v>3.74</v>
+      </c>
+      <c r="V24" t="s">
+        <v>31</v>
+      </c>
+      <c r="W24" t="s">
+        <v>31</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="s">
         <v>32</v>
-      </c>
-      <c r="S24">
-        <v>0.5</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>3</v>
-      </c>
-      <c r="V24">
-        <v>10</v>
-      </c>
-      <c r="W24">
-        <v>3.74</v>
-      </c>
-      <c r="X24">
-        <v>3.74</v>
-      </c>
-      <c r="Y24">
-        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -2524,40 +2524,40 @@
         <v>-2.5</v>
       </c>
       <c r="N25">
-        <v>3.74</v>
-      </c>
-      <c r="O25" t="s">
-        <v>31</v>
-      </c>
-      <c r="P25" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O25">
+        <v>10</v>
+      </c>
+      <c r="P25">
+        <v>3.74</v>
       </c>
       <c r="Q25" t="s">
         <v>31</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25">
+        <v>0.5</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>3.74</v>
+      </c>
+      <c r="U25">
+        <v>3.74</v>
+      </c>
+      <c r="V25" t="s">
+        <v>31</v>
+      </c>
+      <c r="W25" t="s">
+        <v>31</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25" t="s">
         <v>32</v>
-      </c>
-      <c r="S25">
-        <v>0.5</v>
-      </c>
-      <c r="T25">
-        <v>0</v>
-      </c>
-      <c r="U25">
-        <v>3</v>
-      </c>
-      <c r="V25">
-        <v>10</v>
-      </c>
-      <c r="W25">
-        <v>3.74</v>
-      </c>
-      <c r="X25">
-        <v>3.74</v>
-      </c>
-      <c r="Y25">
-        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -2601,40 +2601,40 @@
         <v>-2.5</v>
       </c>
       <c r="N26">
-        <v>3.74</v>
-      </c>
-      <c r="O26" t="s">
-        <v>31</v>
-      </c>
-      <c r="P26" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O26">
+        <v>10</v>
+      </c>
+      <c r="P26">
+        <v>3.74</v>
       </c>
       <c r="Q26" t="s">
         <v>31</v>
       </c>
-      <c r="R26" t="s">
+      <c r="R26">
+        <v>0.5</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>3.74</v>
+      </c>
+      <c r="U26">
+        <v>3.74</v>
+      </c>
+      <c r="V26" t="s">
+        <v>31</v>
+      </c>
+      <c r="W26" t="s">
+        <v>31</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="s">
         <v>32</v>
-      </c>
-      <c r="S26">
-        <v>0.5</v>
-      </c>
-      <c r="T26">
-        <v>0</v>
-      </c>
-      <c r="U26">
-        <v>3</v>
-      </c>
-      <c r="V26">
-        <v>10</v>
-      </c>
-      <c r="W26">
-        <v>3.74</v>
-      </c>
-      <c r="X26">
-        <v>3.74</v>
-      </c>
-      <c r="Y26">
-        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -2678,40 +2678,40 @@
         <v>-2.5</v>
       </c>
       <c r="N27">
-        <v>3.74</v>
-      </c>
-      <c r="O27" t="s">
-        <v>31</v>
-      </c>
-      <c r="P27" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O27">
+        <v>10</v>
+      </c>
+      <c r="P27">
+        <v>3.74</v>
       </c>
       <c r="Q27" t="s">
         <v>31</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R27">
+        <v>0.5</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>3.74</v>
+      </c>
+      <c r="U27">
+        <v>3.74</v>
+      </c>
+      <c r="V27" t="s">
+        <v>31</v>
+      </c>
+      <c r="W27" t="s">
+        <v>31</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="s">
         <v>32</v>
-      </c>
-      <c r="S27">
-        <v>0.5</v>
-      </c>
-      <c r="T27">
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <v>3</v>
-      </c>
-      <c r="V27">
-        <v>10</v>
-      </c>
-      <c r="W27">
-        <v>3.74</v>
-      </c>
-      <c r="X27">
-        <v>3.74</v>
-      </c>
-      <c r="Y27">
-        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -2755,40 +2755,40 @@
         <v>-2.5</v>
       </c>
       <c r="N28">
-        <v>3.74</v>
-      </c>
-      <c r="O28" t="s">
-        <v>31</v>
-      </c>
-      <c r="P28" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O28">
+        <v>10</v>
+      </c>
+      <c r="P28">
+        <v>3.74</v>
       </c>
       <c r="Q28" t="s">
         <v>31</v>
       </c>
-      <c r="R28" t="s">
+      <c r="R28">
+        <v>0.5</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>3.74</v>
+      </c>
+      <c r="U28">
+        <v>3.74</v>
+      </c>
+      <c r="V28" t="s">
+        <v>31</v>
+      </c>
+      <c r="W28" t="s">
+        <v>31</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="s">
         <v>32</v>
-      </c>
-      <c r="S28">
-        <v>0.5</v>
-      </c>
-      <c r="T28">
-        <v>0</v>
-      </c>
-      <c r="U28">
-        <v>3</v>
-      </c>
-      <c r="V28">
-        <v>10</v>
-      </c>
-      <c r="W28">
-        <v>3.74</v>
-      </c>
-      <c r="X28">
-        <v>3.74</v>
-      </c>
-      <c r="Y28">
-        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -2832,40 +2832,40 @@
         <v>-2.5</v>
       </c>
       <c r="N29">
-        <v>3.74</v>
-      </c>
-      <c r="O29" t="s">
-        <v>31</v>
-      </c>
-      <c r="P29" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O29">
+        <v>10</v>
+      </c>
+      <c r="P29">
+        <v>3.74</v>
       </c>
       <c r="Q29" t="s">
         <v>31</v>
       </c>
-      <c r="R29" t="s">
+      <c r="R29">
+        <v>0.5</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>3.74</v>
+      </c>
+      <c r="U29">
+        <v>3.74</v>
+      </c>
+      <c r="V29" t="s">
+        <v>31</v>
+      </c>
+      <c r="W29" t="s">
+        <v>31</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="s">
         <v>32</v>
-      </c>
-      <c r="S29">
-        <v>0.5</v>
-      </c>
-      <c r="T29">
-        <v>0</v>
-      </c>
-      <c r="U29">
-        <v>3</v>
-      </c>
-      <c r="V29">
-        <v>10</v>
-      </c>
-      <c r="W29">
-        <v>3.74</v>
-      </c>
-      <c r="X29">
-        <v>3.74</v>
-      </c>
-      <c r="Y29">
-        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -2909,40 +2909,40 @@
         <v>-2.5</v>
       </c>
       <c r="N30">
-        <v>3.74</v>
-      </c>
-      <c r="O30" t="s">
-        <v>31</v>
-      </c>
-      <c r="P30" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O30">
+        <v>10</v>
+      </c>
+      <c r="P30">
+        <v>3.74</v>
       </c>
       <c r="Q30" t="s">
         <v>31</v>
       </c>
-      <c r="R30" t="s">
+      <c r="R30">
+        <v>0.5</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>3.74</v>
+      </c>
+      <c r="U30">
+        <v>3.74</v>
+      </c>
+      <c r="V30" t="s">
+        <v>31</v>
+      </c>
+      <c r="W30" t="s">
+        <v>31</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30" t="s">
         <v>32</v>
-      </c>
-      <c r="S30">
-        <v>0.5</v>
-      </c>
-      <c r="T30">
-        <v>0</v>
-      </c>
-      <c r="U30">
-        <v>3</v>
-      </c>
-      <c r="V30">
-        <v>10</v>
-      </c>
-      <c r="W30">
-        <v>3.74</v>
-      </c>
-      <c r="X30">
-        <v>3.74</v>
-      </c>
-      <c r="Y30">
-        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -2986,40 +2986,40 @@
         <v>-2.5</v>
       </c>
       <c r="N31">
-        <v>3.74</v>
-      </c>
-      <c r="O31" t="s">
-        <v>31</v>
-      </c>
-      <c r="P31" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="O31">
+        <v>10</v>
+      </c>
+      <c r="P31">
+        <v>3.74</v>
       </c>
       <c r="Q31" t="s">
         <v>31</v>
       </c>
-      <c r="R31" t="s">
+      <c r="R31">
+        <v>0.5</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>3.74</v>
+      </c>
+      <c r="U31">
+        <v>3.74</v>
+      </c>
+      <c r="V31" t="s">
+        <v>31</v>
+      </c>
+      <c r="W31" t="s">
+        <v>31</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31" t="s">
         <v>32</v>
-      </c>
-      <c r="S31">
-        <v>0.5</v>
-      </c>
-      <c r="T31">
-        <v>0</v>
-      </c>
-      <c r="U31">
-        <v>3</v>
-      </c>
-      <c r="V31">
-        <v>10</v>
-      </c>
-      <c r="W31">
-        <v>3.74</v>
-      </c>
-      <c r="X31">
-        <v>3.74</v>
-      </c>
-      <c r="Y31">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new files created post build and Go 1.7 update
</commit_message>
<xml_diff>
--- a/antha/examples/workflows/AccuracyTest/AccuracytestPostMixHVoutput_test.xlsx
+++ b/antha/examples/workflows/AccuracyTest/AccuracytestPostMixHVoutput_test.xlsx
@@ -57,42 +57,42 @@
     <t>Plate WellYStart</t>
   </si>
   <si>
+    <t>LHPolicy_DSPREFERENCE</t>
+  </si>
+  <si>
+    <t>LHPolicy_POST_MIX_VOLUME</t>
+  </si>
+  <si>
+    <t>LHPolicy_POST_MIX_RATE</t>
+  </si>
+  <si>
+    <t>LHPolicy_ASPSPEED</t>
+  </si>
+  <si>
+    <t>LHPolicy_CAN_SDD</t>
+  </si>
+  <si>
+    <t>LHPolicy_DSPZOFFSET</t>
+  </si>
+  <si>
+    <t>LHPolicy_TIP_REUSE_LIMIT</t>
+  </si>
+  <si>
+    <t>LHPolicy_NO_AIR_DISPENSE</t>
+  </si>
+  <si>
     <t>LHPolicy_POST_MIX</t>
   </si>
   <si>
-    <t>LHPolicy_POST_MIX_VOLUME</t>
-  </si>
-  <si>
-    <t>LHPolicy_ASPSPEED</t>
+    <t>LHPolicy_DSPSPEED</t>
+  </si>
+  <si>
+    <t>LHPolicy_CAN_MULTI</t>
   </si>
   <si>
     <t>LHPolicy_CAN_MSA</t>
   </si>
   <si>
-    <t>LHPolicy_DSPZOFFSET</t>
-  </si>
-  <si>
-    <t>LHPolicy_TIP_REUSE_LIMIT</t>
-  </si>
-  <si>
-    <t>LHPolicy_POST_MIX_RATE</t>
-  </si>
-  <si>
-    <t>LHPolicy_DSPSPEED</t>
-  </si>
-  <si>
-    <t>LHPolicy_CAN_MULTI</t>
-  </si>
-  <si>
-    <t>LHPolicy_CAN_SDD</t>
-  </si>
-  <si>
-    <t>LHPolicy_DSPREFERENCE</t>
-  </si>
-  <si>
-    <t>LHPolicy_NO_AIR_DISPENSE</t>
-  </si>
-  <si>
     <t>tartrazine</t>
   </si>
   <si>
@@ -102,7 +102,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>E10</t>
+    <t>D10</t>
   </si>
   <si>
     <t>PostMix</t>
@@ -120,115 +120,115 @@
     <t>2</t>
   </si>
   <si>
-    <t>L4</t>
+    <t>J8</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>L7</t>
+    <t>K12</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>M4</t>
+    <t>M9</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>I12</t>
+    <t>O13</t>
   </si>
   <si>
     <t>30.000ul</t>
   </si>
   <si>
-    <t>N5</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
-    <t>N11</t>
-  </si>
-  <si>
-    <t>F15</t>
-  </si>
-  <si>
-    <t>N8</t>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>M11</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>K10</t>
+  </si>
+  <si>
+    <t>H5</t>
   </si>
   <si>
     <t>35.000ul</t>
   </si>
   <si>
-    <t>P13</t>
-  </si>
-  <si>
-    <t>I4</t>
-  </si>
-  <si>
-    <t>L8</t>
-  </si>
-  <si>
-    <t>M12</t>
-  </si>
-  <si>
-    <t>M14</t>
+    <t>N12</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>F7</t>
   </si>
   <si>
     <t>40.000ul</t>
   </si>
   <si>
-    <t>O14</t>
-  </si>
-  <si>
-    <t>K13</t>
-  </si>
-  <si>
-    <t>H4</t>
-  </si>
-  <si>
-    <t>I13</t>
-  </si>
-  <si>
-    <t>J6</t>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>N9</t>
   </si>
   <si>
     <t>45.000ul</t>
   </si>
   <si>
-    <t>F3</t>
-  </si>
-  <si>
-    <t>F5</t>
-  </si>
-  <si>
-    <t>H11</t>
-  </si>
-  <si>
-    <t>I8</t>
-  </si>
-  <si>
-    <t>J10</t>
+    <t>L10</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>G16</t>
+  </si>
+  <si>
+    <t>I6</t>
+  </si>
+  <si>
+    <t>M3</t>
   </si>
   <si>
     <t>50.000ul</t>
   </si>
   <si>
-    <t>O12</t>
+    <t>N6</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>I11</t>
   </si>
   <si>
     <t>E9</t>
   </si>
   <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>H12</t>
+    <t>I5</t>
   </si>
 </sst>
 </file>
@@ -753,7 +753,7 @@
         <v>-2.5</v>
       </c>
       <c r="N2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O2">
         <v>10</v>
@@ -761,32 +761,32 @@
       <c r="P2">
         <v>3.74</v>
       </c>
-      <c r="Q2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2">
+      <c r="Q2">
+        <v>3.74</v>
+      </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2">
         <v>0.5</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
       <c r="T2">
-        <v>3.74</v>
-      </c>
-      <c r="U2">
-        <v>3.74</v>
-      </c>
-      <c r="V2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W2" t="s">
-        <v>31</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2">
+        <v>3</v>
+      </c>
+      <c r="W2">
+        <v>3.74</v>
+      </c>
+      <c r="X2" t="s">
+        <v>31</v>
       </c>
       <c r="Y2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -830,7 +830,7 @@
         <v>-2.5</v>
       </c>
       <c r="N3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O3">
         <v>10</v>
@@ -838,32 +838,32 @@
       <c r="P3">
         <v>3.74</v>
       </c>
-      <c r="Q3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3">
+      <c r="Q3">
+        <v>3.74</v>
+      </c>
+      <c r="R3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3">
         <v>0.5</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
       <c r="T3">
-        <v>3.74</v>
-      </c>
-      <c r="U3">
-        <v>3.74</v>
-      </c>
-      <c r="V3" t="s">
-        <v>31</v>
-      </c>
-      <c r="W3" t="s">
-        <v>31</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>3.74</v>
+      </c>
+      <c r="X3" t="s">
+        <v>31</v>
       </c>
       <c r="Y3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
@@ -907,7 +907,7 @@
         <v>-2.5</v>
       </c>
       <c r="N4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <v>10</v>
@@ -915,32 +915,32 @@
       <c r="P4">
         <v>3.74</v>
       </c>
-      <c r="Q4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R4">
+      <c r="Q4">
+        <v>3.74</v>
+      </c>
+      <c r="R4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4">
         <v>0.5</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
       <c r="T4">
-        <v>3.74</v>
-      </c>
-      <c r="U4">
-        <v>3.74</v>
-      </c>
-      <c r="V4" t="s">
-        <v>31</v>
-      </c>
-      <c r="W4" t="s">
-        <v>31</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="W4">
+        <v>3.74</v>
+      </c>
+      <c r="X4" t="s">
+        <v>31</v>
       </c>
       <c r="Y4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
@@ -984,7 +984,7 @@
         <v>-2.5</v>
       </c>
       <c r="N5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O5">
         <v>10</v>
@@ -992,32 +992,32 @@
       <c r="P5">
         <v>3.74</v>
       </c>
-      <c r="Q5" t="s">
-        <v>31</v>
-      </c>
-      <c r="R5">
+      <c r="Q5">
+        <v>3.74</v>
+      </c>
+      <c r="R5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5">
         <v>0.5</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
       <c r="T5">
-        <v>3.74</v>
-      </c>
-      <c r="U5">
-        <v>3.74</v>
-      </c>
-      <c r="V5" t="s">
-        <v>31</v>
-      </c>
-      <c r="W5" t="s">
-        <v>31</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5">
+        <v>3.74</v>
+      </c>
+      <c r="X5" t="s">
+        <v>31</v>
       </c>
       <c r="Y5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
@@ -1061,7 +1061,7 @@
         <v>-2.5</v>
       </c>
       <c r="N6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <v>10</v>
@@ -1069,32 +1069,32 @@
       <c r="P6">
         <v>3.74</v>
       </c>
-      <c r="Q6" t="s">
-        <v>31</v>
-      </c>
-      <c r="R6">
+      <c r="Q6">
+        <v>3.74</v>
+      </c>
+      <c r="R6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6">
         <v>0.5</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
       <c r="T6">
-        <v>3.74</v>
-      </c>
-      <c r="U6">
-        <v>3.74</v>
-      </c>
-      <c r="V6" t="s">
-        <v>31</v>
-      </c>
-      <c r="W6" t="s">
-        <v>31</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
+        <v>32</v>
+      </c>
+      <c r="V6">
+        <v>3</v>
+      </c>
+      <c r="W6">
+        <v>3.74</v>
+      </c>
+      <c r="X6" t="s">
+        <v>31</v>
       </c>
       <c r="Y6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
@@ -1138,7 +1138,7 @@
         <v>-2.5</v>
       </c>
       <c r="N7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <v>10</v>
@@ -1146,32 +1146,32 @@
       <c r="P7">
         <v>3.74</v>
       </c>
-      <c r="Q7" t="s">
-        <v>31</v>
-      </c>
-      <c r="R7">
+      <c r="Q7">
+        <v>3.74</v>
+      </c>
+      <c r="R7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S7">
         <v>0.5</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
       <c r="T7">
-        <v>3.74</v>
-      </c>
-      <c r="U7">
-        <v>3.74</v>
-      </c>
-      <c r="V7" t="s">
-        <v>31</v>
-      </c>
-      <c r="W7" t="s">
-        <v>31</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U7" t="s">
+        <v>32</v>
+      </c>
+      <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>3.74</v>
+      </c>
+      <c r="X7" t="s">
+        <v>31</v>
       </c>
       <c r="Y7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -1215,7 +1215,7 @@
         <v>-2.5</v>
       </c>
       <c r="N8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>10</v>
@@ -1223,32 +1223,32 @@
       <c r="P8">
         <v>3.74</v>
       </c>
-      <c r="Q8" t="s">
-        <v>31</v>
-      </c>
-      <c r="R8">
+      <c r="Q8">
+        <v>3.74</v>
+      </c>
+      <c r="R8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S8">
         <v>0.5</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
       <c r="T8">
-        <v>3.74</v>
-      </c>
-      <c r="U8">
-        <v>3.74</v>
-      </c>
-      <c r="V8" t="s">
-        <v>31</v>
-      </c>
-      <c r="W8" t="s">
-        <v>31</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V8">
+        <v>3</v>
+      </c>
+      <c r="W8">
+        <v>3.74</v>
+      </c>
+      <c r="X8" t="s">
+        <v>31</v>
       </c>
       <c r="Y8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
@@ -1292,7 +1292,7 @@
         <v>-2.5</v>
       </c>
       <c r="N9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>10</v>
@@ -1300,32 +1300,32 @@
       <c r="P9">
         <v>3.74</v>
       </c>
-      <c r="Q9" t="s">
-        <v>31</v>
-      </c>
-      <c r="R9">
+      <c r="Q9">
+        <v>3.74</v>
+      </c>
+      <c r="R9" t="s">
+        <v>31</v>
+      </c>
+      <c r="S9">
         <v>0.5</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
       <c r="T9">
-        <v>3.74</v>
-      </c>
-      <c r="U9">
-        <v>3.74</v>
-      </c>
-      <c r="V9" t="s">
-        <v>31</v>
-      </c>
-      <c r="W9" t="s">
-        <v>31</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U9" t="s">
+        <v>32</v>
+      </c>
+      <c r="V9">
+        <v>3</v>
+      </c>
+      <c r="W9">
+        <v>3.74</v>
+      </c>
+      <c r="X9" t="s">
+        <v>31</v>
       </c>
       <c r="Y9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
@@ -1369,7 +1369,7 @@
         <v>-2.5</v>
       </c>
       <c r="N10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O10">
         <v>10</v>
@@ -1377,32 +1377,32 @@
       <c r="P10">
         <v>3.74</v>
       </c>
-      <c r="Q10" t="s">
-        <v>31</v>
-      </c>
-      <c r="R10">
+      <c r="Q10">
+        <v>3.74</v>
+      </c>
+      <c r="R10" t="s">
+        <v>31</v>
+      </c>
+      <c r="S10">
         <v>0.5</v>
       </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
       <c r="T10">
-        <v>3.74</v>
-      </c>
-      <c r="U10">
-        <v>3.74</v>
-      </c>
-      <c r="V10" t="s">
-        <v>31</v>
-      </c>
-      <c r="W10" t="s">
-        <v>31</v>
-      </c>
-      <c r="X10">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U10" t="s">
+        <v>32</v>
+      </c>
+      <c r="V10">
+        <v>3</v>
+      </c>
+      <c r="W10">
+        <v>3.74</v>
+      </c>
+      <c r="X10" t="s">
+        <v>31</v>
       </c>
       <c r="Y10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -1446,7 +1446,7 @@
         <v>-2.5</v>
       </c>
       <c r="N11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <v>10</v>
@@ -1454,32 +1454,32 @@
       <c r="P11">
         <v>3.74</v>
       </c>
-      <c r="Q11" t="s">
-        <v>31</v>
-      </c>
-      <c r="R11">
+      <c r="Q11">
+        <v>3.74</v>
+      </c>
+      <c r="R11" t="s">
+        <v>31</v>
+      </c>
+      <c r="S11">
         <v>0.5</v>
       </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
       <c r="T11">
-        <v>3.74</v>
-      </c>
-      <c r="U11">
-        <v>3.74</v>
-      </c>
-      <c r="V11" t="s">
-        <v>31</v>
-      </c>
-      <c r="W11" t="s">
-        <v>31</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U11" t="s">
+        <v>32</v>
+      </c>
+      <c r="V11">
+        <v>3</v>
+      </c>
+      <c r="W11">
+        <v>3.74</v>
+      </c>
+      <c r="X11" t="s">
+        <v>31</v>
       </c>
       <c r="Y11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12">
@@ -1523,7 +1523,7 @@
         <v>-2.5</v>
       </c>
       <c r="N12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <v>10</v>
@@ -1531,32 +1531,32 @@
       <c r="P12">
         <v>3.74</v>
       </c>
-      <c r="Q12" t="s">
-        <v>31</v>
-      </c>
-      <c r="R12">
+      <c r="Q12">
+        <v>3.74</v>
+      </c>
+      <c r="R12" t="s">
+        <v>31</v>
+      </c>
+      <c r="S12">
         <v>0.5</v>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
       <c r="T12">
-        <v>3.74</v>
-      </c>
-      <c r="U12">
-        <v>3.74</v>
-      </c>
-      <c r="V12" t="s">
-        <v>31</v>
-      </c>
-      <c r="W12" t="s">
-        <v>31</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U12" t="s">
+        <v>32</v>
+      </c>
+      <c r="V12">
+        <v>3</v>
+      </c>
+      <c r="W12">
+        <v>3.74</v>
+      </c>
+      <c r="X12" t="s">
+        <v>31</v>
       </c>
       <c r="Y12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
@@ -1600,7 +1600,7 @@
         <v>-2.5</v>
       </c>
       <c r="N13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O13">
         <v>10</v>
@@ -1608,32 +1608,32 @@
       <c r="P13">
         <v>3.74</v>
       </c>
-      <c r="Q13" t="s">
-        <v>31</v>
-      </c>
-      <c r="R13">
+      <c r="Q13">
+        <v>3.74</v>
+      </c>
+      <c r="R13" t="s">
+        <v>31</v>
+      </c>
+      <c r="S13">
         <v>0.5</v>
       </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
       <c r="T13">
-        <v>3.74</v>
-      </c>
-      <c r="U13">
-        <v>3.74</v>
-      </c>
-      <c r="V13" t="s">
-        <v>31</v>
-      </c>
-      <c r="W13" t="s">
-        <v>31</v>
-      </c>
-      <c r="X13">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
+        <v>32</v>
+      </c>
+      <c r="V13">
+        <v>3</v>
+      </c>
+      <c r="W13">
+        <v>3.74</v>
+      </c>
+      <c r="X13" t="s">
+        <v>31</v>
       </c>
       <c r="Y13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
@@ -1677,7 +1677,7 @@
         <v>-2.5</v>
       </c>
       <c r="N14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O14">
         <v>10</v>
@@ -1685,32 +1685,32 @@
       <c r="P14">
         <v>3.74</v>
       </c>
-      <c r="Q14" t="s">
-        <v>31</v>
-      </c>
-      <c r="R14">
+      <c r="Q14">
+        <v>3.74</v>
+      </c>
+      <c r="R14" t="s">
+        <v>31</v>
+      </c>
+      <c r="S14">
         <v>0.5</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
       <c r="T14">
-        <v>3.74</v>
-      </c>
-      <c r="U14">
-        <v>3.74</v>
-      </c>
-      <c r="V14" t="s">
-        <v>31</v>
-      </c>
-      <c r="W14" t="s">
-        <v>31</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
+        <v>32</v>
+      </c>
+      <c r="V14">
+        <v>3</v>
+      </c>
+      <c r="W14">
+        <v>3.74</v>
+      </c>
+      <c r="X14" t="s">
+        <v>31</v>
       </c>
       <c r="Y14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15">
@@ -1754,7 +1754,7 @@
         <v>-2.5</v>
       </c>
       <c r="N15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O15">
         <v>10</v>
@@ -1762,32 +1762,32 @@
       <c r="P15">
         <v>3.74</v>
       </c>
-      <c r="Q15" t="s">
-        <v>31</v>
-      </c>
-      <c r="R15">
+      <c r="Q15">
+        <v>3.74</v>
+      </c>
+      <c r="R15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S15">
         <v>0.5</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
       <c r="T15">
-        <v>3.74</v>
-      </c>
-      <c r="U15">
-        <v>3.74</v>
-      </c>
-      <c r="V15" t="s">
-        <v>31</v>
-      </c>
-      <c r="W15" t="s">
-        <v>31</v>
-      </c>
-      <c r="X15">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U15" t="s">
+        <v>32</v>
+      </c>
+      <c r="V15">
+        <v>3</v>
+      </c>
+      <c r="W15">
+        <v>3.74</v>
+      </c>
+      <c r="X15" t="s">
+        <v>31</v>
       </c>
       <c r="Y15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16">
@@ -1831,7 +1831,7 @@
         <v>-2.5</v>
       </c>
       <c r="N16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O16">
         <v>10</v>
@@ -1839,32 +1839,32 @@
       <c r="P16">
         <v>3.74</v>
       </c>
-      <c r="Q16" t="s">
-        <v>31</v>
-      </c>
-      <c r="R16">
+      <c r="Q16">
+        <v>3.74</v>
+      </c>
+      <c r="R16" t="s">
+        <v>31</v>
+      </c>
+      <c r="S16">
         <v>0.5</v>
       </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
       <c r="T16">
-        <v>3.74</v>
-      </c>
-      <c r="U16">
-        <v>3.74</v>
-      </c>
-      <c r="V16" t="s">
-        <v>31</v>
-      </c>
-      <c r="W16" t="s">
-        <v>31</v>
-      </c>
-      <c r="X16">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U16" t="s">
+        <v>32</v>
+      </c>
+      <c r="V16">
+        <v>3</v>
+      </c>
+      <c r="W16">
+        <v>3.74</v>
+      </c>
+      <c r="X16" t="s">
+        <v>31</v>
       </c>
       <c r="Y16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17">
@@ -1908,7 +1908,7 @@
         <v>-2.5</v>
       </c>
       <c r="N17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O17">
         <v>10</v>
@@ -1916,32 +1916,32 @@
       <c r="P17">
         <v>3.74</v>
       </c>
-      <c r="Q17" t="s">
-        <v>31</v>
-      </c>
-      <c r="R17">
+      <c r="Q17">
+        <v>3.74</v>
+      </c>
+      <c r="R17" t="s">
+        <v>31</v>
+      </c>
+      <c r="S17">
         <v>0.5</v>
       </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
       <c r="T17">
-        <v>3.74</v>
-      </c>
-      <c r="U17">
-        <v>3.74</v>
-      </c>
-      <c r="V17" t="s">
-        <v>31</v>
-      </c>
-      <c r="W17" t="s">
-        <v>31</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U17" t="s">
+        <v>32</v>
+      </c>
+      <c r="V17">
+        <v>3</v>
+      </c>
+      <c r="W17">
+        <v>3.74</v>
+      </c>
+      <c r="X17" t="s">
+        <v>31</v>
       </c>
       <c r="Y17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18">
@@ -1985,7 +1985,7 @@
         <v>-2.5</v>
       </c>
       <c r="N18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O18">
         <v>10</v>
@@ -1993,32 +1993,32 @@
       <c r="P18">
         <v>3.74</v>
       </c>
-      <c r="Q18" t="s">
-        <v>31</v>
-      </c>
-      <c r="R18">
+      <c r="Q18">
+        <v>3.74</v>
+      </c>
+      <c r="R18" t="s">
+        <v>31</v>
+      </c>
+      <c r="S18">
         <v>0.5</v>
       </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
       <c r="T18">
-        <v>3.74</v>
-      </c>
-      <c r="U18">
-        <v>3.74</v>
-      </c>
-      <c r="V18" t="s">
-        <v>31</v>
-      </c>
-      <c r="W18" t="s">
-        <v>31</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U18" t="s">
+        <v>32</v>
+      </c>
+      <c r="V18">
+        <v>3</v>
+      </c>
+      <c r="W18">
+        <v>3.74</v>
+      </c>
+      <c r="X18" t="s">
+        <v>31</v>
       </c>
       <c r="Y18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19">
@@ -2062,7 +2062,7 @@
         <v>-2.5</v>
       </c>
       <c r="N19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O19">
         <v>10</v>
@@ -2070,32 +2070,32 @@
       <c r="P19">
         <v>3.74</v>
       </c>
-      <c r="Q19" t="s">
-        <v>31</v>
-      </c>
-      <c r="R19">
+      <c r="Q19">
+        <v>3.74</v>
+      </c>
+      <c r="R19" t="s">
+        <v>31</v>
+      </c>
+      <c r="S19">
         <v>0.5</v>
       </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
       <c r="T19">
-        <v>3.74</v>
-      </c>
-      <c r="U19">
-        <v>3.74</v>
-      </c>
-      <c r="V19" t="s">
-        <v>31</v>
-      </c>
-      <c r="W19" t="s">
-        <v>31</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U19" t="s">
+        <v>32</v>
+      </c>
+      <c r="V19">
+        <v>3</v>
+      </c>
+      <c r="W19">
+        <v>3.74</v>
+      </c>
+      <c r="X19" t="s">
+        <v>31</v>
       </c>
       <c r="Y19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20">
@@ -2139,7 +2139,7 @@
         <v>-2.5</v>
       </c>
       <c r="N20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O20">
         <v>10</v>
@@ -2147,32 +2147,32 @@
       <c r="P20">
         <v>3.74</v>
       </c>
-      <c r="Q20" t="s">
-        <v>31</v>
-      </c>
-      <c r="R20">
+      <c r="Q20">
+        <v>3.74</v>
+      </c>
+      <c r="R20" t="s">
+        <v>31</v>
+      </c>
+      <c r="S20">
         <v>0.5</v>
       </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
       <c r="T20">
-        <v>3.74</v>
-      </c>
-      <c r="U20">
-        <v>3.74</v>
-      </c>
-      <c r="V20" t="s">
-        <v>31</v>
-      </c>
-      <c r="W20" t="s">
-        <v>31</v>
-      </c>
-      <c r="X20">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U20" t="s">
+        <v>32</v>
+      </c>
+      <c r="V20">
+        <v>3</v>
+      </c>
+      <c r="W20">
+        <v>3.74</v>
+      </c>
+      <c r="X20" t="s">
+        <v>31</v>
       </c>
       <c r="Y20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21">
@@ -2216,7 +2216,7 @@
         <v>-2.5</v>
       </c>
       <c r="N21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O21">
         <v>10</v>
@@ -2224,32 +2224,32 @@
       <c r="P21">
         <v>3.74</v>
       </c>
-      <c r="Q21" t="s">
-        <v>31</v>
-      </c>
-      <c r="R21">
+      <c r="Q21">
+        <v>3.74</v>
+      </c>
+      <c r="R21" t="s">
+        <v>31</v>
+      </c>
+      <c r="S21">
         <v>0.5</v>
       </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
       <c r="T21">
-        <v>3.74</v>
-      </c>
-      <c r="U21">
-        <v>3.74</v>
-      </c>
-      <c r="V21" t="s">
-        <v>31</v>
-      </c>
-      <c r="W21" t="s">
-        <v>31</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U21" t="s">
+        <v>32</v>
+      </c>
+      <c r="V21">
+        <v>3</v>
+      </c>
+      <c r="W21">
+        <v>3.74</v>
+      </c>
+      <c r="X21" t="s">
+        <v>31</v>
       </c>
       <c r="Y21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22">
@@ -2293,7 +2293,7 @@
         <v>-2.5</v>
       </c>
       <c r="N22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <v>10</v>
@@ -2301,32 +2301,32 @@
       <c r="P22">
         <v>3.74</v>
       </c>
-      <c r="Q22" t="s">
-        <v>31</v>
-      </c>
-      <c r="R22">
+      <c r="Q22">
+        <v>3.74</v>
+      </c>
+      <c r="R22" t="s">
+        <v>31</v>
+      </c>
+      <c r="S22">
         <v>0.5</v>
       </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
       <c r="T22">
-        <v>3.74</v>
-      </c>
-      <c r="U22">
-        <v>3.74</v>
-      </c>
-      <c r="V22" t="s">
-        <v>31</v>
-      </c>
-      <c r="W22" t="s">
-        <v>31</v>
-      </c>
-      <c r="X22">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U22" t="s">
+        <v>32</v>
+      </c>
+      <c r="V22">
+        <v>3</v>
+      </c>
+      <c r="W22">
+        <v>3.74</v>
+      </c>
+      <c r="X22" t="s">
+        <v>31</v>
       </c>
       <c r="Y22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23">
@@ -2370,7 +2370,7 @@
         <v>-2.5</v>
       </c>
       <c r="N23">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O23">
         <v>10</v>
@@ -2378,32 +2378,32 @@
       <c r="P23">
         <v>3.74</v>
       </c>
-      <c r="Q23" t="s">
-        <v>31</v>
-      </c>
-      <c r="R23">
+      <c r="Q23">
+        <v>3.74</v>
+      </c>
+      <c r="R23" t="s">
+        <v>31</v>
+      </c>
+      <c r="S23">
         <v>0.5</v>
       </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
       <c r="T23">
-        <v>3.74</v>
-      </c>
-      <c r="U23">
-        <v>3.74</v>
-      </c>
-      <c r="V23" t="s">
-        <v>31</v>
-      </c>
-      <c r="W23" t="s">
-        <v>31</v>
-      </c>
-      <c r="X23">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U23" t="s">
+        <v>32</v>
+      </c>
+      <c r="V23">
+        <v>3</v>
+      </c>
+      <c r="W23">
+        <v>3.74</v>
+      </c>
+      <c r="X23" t="s">
+        <v>31</v>
       </c>
       <c r="Y23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24">
@@ -2447,7 +2447,7 @@
         <v>-2.5</v>
       </c>
       <c r="N24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O24">
         <v>10</v>
@@ -2455,32 +2455,32 @@
       <c r="P24">
         <v>3.74</v>
       </c>
-      <c r="Q24" t="s">
-        <v>31</v>
-      </c>
-      <c r="R24">
+      <c r="Q24">
+        <v>3.74</v>
+      </c>
+      <c r="R24" t="s">
+        <v>31</v>
+      </c>
+      <c r="S24">
         <v>0.5</v>
       </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
       <c r="T24">
-        <v>3.74</v>
-      </c>
-      <c r="U24">
-        <v>3.74</v>
-      </c>
-      <c r="V24" t="s">
-        <v>31</v>
-      </c>
-      <c r="W24" t="s">
-        <v>31</v>
-      </c>
-      <c r="X24">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U24" t="s">
+        <v>32</v>
+      </c>
+      <c r="V24">
+        <v>3</v>
+      </c>
+      <c r="W24">
+        <v>3.74</v>
+      </c>
+      <c r="X24" t="s">
+        <v>31</v>
       </c>
       <c r="Y24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25">
@@ -2524,7 +2524,7 @@
         <v>-2.5</v>
       </c>
       <c r="N25">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O25">
         <v>10</v>
@@ -2532,32 +2532,32 @@
       <c r="P25">
         <v>3.74</v>
       </c>
-      <c r="Q25" t="s">
-        <v>31</v>
-      </c>
-      <c r="R25">
+      <c r="Q25">
+        <v>3.74</v>
+      </c>
+      <c r="R25" t="s">
+        <v>31</v>
+      </c>
+      <c r="S25">
         <v>0.5</v>
       </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
       <c r="T25">
-        <v>3.74</v>
-      </c>
-      <c r="U25">
-        <v>3.74</v>
-      </c>
-      <c r="V25" t="s">
-        <v>31</v>
-      </c>
-      <c r="W25" t="s">
-        <v>31</v>
-      </c>
-      <c r="X25">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U25" t="s">
+        <v>32</v>
+      </c>
+      <c r="V25">
+        <v>3</v>
+      </c>
+      <c r="W25">
+        <v>3.74</v>
+      </c>
+      <c r="X25" t="s">
+        <v>31</v>
       </c>
       <c r="Y25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26">
@@ -2601,7 +2601,7 @@
         <v>-2.5</v>
       </c>
       <c r="N26">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O26">
         <v>10</v>
@@ -2609,32 +2609,32 @@
       <c r="P26">
         <v>3.74</v>
       </c>
-      <c r="Q26" t="s">
-        <v>31</v>
-      </c>
-      <c r="R26">
+      <c r="Q26">
+        <v>3.74</v>
+      </c>
+      <c r="R26" t="s">
+        <v>31</v>
+      </c>
+      <c r="S26">
         <v>0.5</v>
       </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
       <c r="T26">
-        <v>3.74</v>
-      </c>
-      <c r="U26">
-        <v>3.74</v>
-      </c>
-      <c r="V26" t="s">
-        <v>31</v>
-      </c>
-      <c r="W26" t="s">
-        <v>31</v>
-      </c>
-      <c r="X26">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U26" t="s">
+        <v>32</v>
+      </c>
+      <c r="V26">
+        <v>3</v>
+      </c>
+      <c r="W26">
+        <v>3.74</v>
+      </c>
+      <c r="X26" t="s">
+        <v>31</v>
       </c>
       <c r="Y26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27">
@@ -2678,7 +2678,7 @@
         <v>-2.5</v>
       </c>
       <c r="N27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O27">
         <v>10</v>
@@ -2686,32 +2686,32 @@
       <c r="P27">
         <v>3.74</v>
       </c>
-      <c r="Q27" t="s">
-        <v>31</v>
-      </c>
-      <c r="R27">
+      <c r="Q27">
+        <v>3.74</v>
+      </c>
+      <c r="R27" t="s">
+        <v>31</v>
+      </c>
+      <c r="S27">
         <v>0.5</v>
       </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
       <c r="T27">
-        <v>3.74</v>
-      </c>
-      <c r="U27">
-        <v>3.74</v>
-      </c>
-      <c r="V27" t="s">
-        <v>31</v>
-      </c>
-      <c r="W27" t="s">
-        <v>31</v>
-      </c>
-      <c r="X27">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U27" t="s">
+        <v>32</v>
+      </c>
+      <c r="V27">
+        <v>3</v>
+      </c>
+      <c r="W27">
+        <v>3.74</v>
+      </c>
+      <c r="X27" t="s">
+        <v>31</v>
       </c>
       <c r="Y27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28">
@@ -2755,7 +2755,7 @@
         <v>-2.5</v>
       </c>
       <c r="N28">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O28">
         <v>10</v>
@@ -2763,32 +2763,32 @@
       <c r="P28">
         <v>3.74</v>
       </c>
-      <c r="Q28" t="s">
-        <v>31</v>
-      </c>
-      <c r="R28">
+      <c r="Q28">
+        <v>3.74</v>
+      </c>
+      <c r="R28" t="s">
+        <v>31</v>
+      </c>
+      <c r="S28">
         <v>0.5</v>
       </c>
-      <c r="S28">
-        <v>0</v>
-      </c>
       <c r="T28">
-        <v>3.74</v>
-      </c>
-      <c r="U28">
-        <v>3.74</v>
-      </c>
-      <c r="V28" t="s">
-        <v>31</v>
-      </c>
-      <c r="W28" t="s">
-        <v>31</v>
-      </c>
-      <c r="X28">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U28" t="s">
+        <v>32</v>
+      </c>
+      <c r="V28">
+        <v>3</v>
+      </c>
+      <c r="W28">
+        <v>3.74</v>
+      </c>
+      <c r="X28" t="s">
+        <v>31</v>
       </c>
       <c r="Y28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29">
@@ -2832,7 +2832,7 @@
         <v>-2.5</v>
       </c>
       <c r="N29">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O29">
         <v>10</v>
@@ -2840,32 +2840,32 @@
       <c r="P29">
         <v>3.74</v>
       </c>
-      <c r="Q29" t="s">
-        <v>31</v>
-      </c>
-      <c r="R29">
+      <c r="Q29">
+        <v>3.74</v>
+      </c>
+      <c r="R29" t="s">
+        <v>31</v>
+      </c>
+      <c r="S29">
         <v>0.5</v>
       </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
       <c r="T29">
-        <v>3.74</v>
-      </c>
-      <c r="U29">
-        <v>3.74</v>
-      </c>
-      <c r="V29" t="s">
-        <v>31</v>
-      </c>
-      <c r="W29" t="s">
-        <v>31</v>
-      </c>
-      <c r="X29">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U29" t="s">
+        <v>32</v>
+      </c>
+      <c r="V29">
+        <v>3</v>
+      </c>
+      <c r="W29">
+        <v>3.74</v>
+      </c>
+      <c r="X29" t="s">
+        <v>31</v>
       </c>
       <c r="Y29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30">
@@ -2909,7 +2909,7 @@
         <v>-2.5</v>
       </c>
       <c r="N30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O30">
         <v>10</v>
@@ -2917,32 +2917,32 @@
       <c r="P30">
         <v>3.74</v>
       </c>
-      <c r="Q30" t="s">
-        <v>31</v>
-      </c>
-      <c r="R30">
+      <c r="Q30">
+        <v>3.74</v>
+      </c>
+      <c r="R30" t="s">
+        <v>31</v>
+      </c>
+      <c r="S30">
         <v>0.5</v>
       </c>
-      <c r="S30">
-        <v>0</v>
-      </c>
       <c r="T30">
-        <v>3.74</v>
-      </c>
-      <c r="U30">
-        <v>3.74</v>
-      </c>
-      <c r="V30" t="s">
-        <v>31</v>
-      </c>
-      <c r="W30" t="s">
-        <v>31</v>
-      </c>
-      <c r="X30">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U30" t="s">
+        <v>32</v>
+      </c>
+      <c r="V30">
+        <v>3</v>
+      </c>
+      <c r="W30">
+        <v>3.74</v>
+      </c>
+      <c r="X30" t="s">
+        <v>31</v>
       </c>
       <c r="Y30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31">
@@ -2986,7 +2986,7 @@
         <v>-2.5</v>
       </c>
       <c r="N31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O31">
         <v>10</v>
@@ -2994,32 +2994,32 @@
       <c r="P31">
         <v>3.74</v>
       </c>
-      <c r="Q31" t="s">
-        <v>31</v>
-      </c>
-      <c r="R31">
+      <c r="Q31">
+        <v>3.74</v>
+      </c>
+      <c r="R31" t="s">
+        <v>31</v>
+      </c>
+      <c r="S31">
         <v>0.5</v>
       </c>
-      <c r="S31">
-        <v>0</v>
-      </c>
       <c r="T31">
-        <v>3.74</v>
-      </c>
-      <c r="U31">
-        <v>3.74</v>
-      </c>
-      <c r="V31" t="s">
-        <v>31</v>
-      </c>
-      <c r="W31" t="s">
-        <v>31</v>
-      </c>
-      <c r="X31">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="U31" t="s">
+        <v>32</v>
+      </c>
+      <c r="V31">
+        <v>3</v>
+      </c>
+      <c r="W31">
+        <v>3.74</v>
+      </c>
+      <c r="X31" t="s">
+        <v>31</v>
       </c>
       <c r="Y31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>